<commit_message>
Add .gitattributes to enforce LF line endings
</commit_message>
<xml_diff>
--- a/IAAPS_Corte_Marzo.xlsx
+++ b/IAAPS_Corte_Marzo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SALUD_CURICO\iaaps-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128F95EB-E565-4D70-8651-64B32B5356A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60950B7D-9EBE-419E-8AA6-A153DB33D1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13749" xr2:uid="{66EFEE98-29CC-4533-B94C-81E7E1EBEEAF}"/>
   </bookViews>
@@ -822,25 +822,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{301DFA57-F574-41A6-870E-2EAA91A7C829}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O402"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G380" sqref="G380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.44140625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="24.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="23" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" style="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.44140625" style="30" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.109375" style="24" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" style="25" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" style="25" customWidth="1"/>
     <col min="12" max="12" width="20.109375" style="26" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="8.44140625" style="7"/>
   </cols>
@@ -903,10 +904,10 @@
         <v>16</v>
       </c>
       <c r="F2" s="10">
-        <v>675</v>
+        <v>15</v>
       </c>
       <c r="G2" s="10">
-        <v>675</v>
+        <v>15</v>
       </c>
       <c r="H2" s="11">
         <v>1</v>
@@ -921,8 +922,7 @@
         <v>0.04</v>
       </c>
       <c r="L2" s="15">
-        <f>100%*100</f>
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -945,10 +945,10 @@
         <v>16</v>
       </c>
       <c r="F3" s="10">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="G3" s="10">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="H3" s="11">
         <v>1</v>
@@ -986,10 +986,10 @@
         <v>16</v>
       </c>
       <c r="F4" s="10">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="G4" s="10">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="H4" s="11">
         <v>1</v>
@@ -1027,10 +1027,10 @@
         <v>16</v>
       </c>
       <c r="F5" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G5" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H5" s="11">
         <v>1</v>
@@ -1068,10 +1068,10 @@
         <v>16</v>
       </c>
       <c r="F6" s="10">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="G6" s="10">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="H6" s="11">
         <v>1</v>
@@ -1109,10 +1109,10 @@
         <v>16</v>
       </c>
       <c r="F7" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G7" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H7" s="11">
         <v>1</v>
@@ -1150,10 +1150,10 @@
         <v>16</v>
       </c>
       <c r="F8" s="10">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="G8" s="10">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="H8" s="11">
         <v>1</v>
@@ -1191,10 +1191,10 @@
         <v>16</v>
       </c>
       <c r="F9" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G9" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H9" s="11">
         <v>1</v>
@@ -1232,10 +1232,10 @@
         <v>16</v>
       </c>
       <c r="F10" s="10">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="G10" s="10">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="H10" s="11">
         <v>1</v>
@@ -1273,10 +1273,10 @@
         <v>16</v>
       </c>
       <c r="F11" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G11" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H11" s="11">
         <v>1</v>
@@ -1314,10 +1314,10 @@
         <v>16</v>
       </c>
       <c r="F12" s="10">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="G12" s="10">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="H12" s="11">
         <v>1</v>
@@ -1355,10 +1355,10 @@
         <v>16</v>
       </c>
       <c r="F13" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G13" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H13" s="11">
         <v>1</v>
@@ -1396,10 +1396,10 @@
         <v>16</v>
       </c>
       <c r="F14" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G14" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H14" s="11">
         <v>1</v>
@@ -1437,10 +1437,10 @@
         <v>16</v>
       </c>
       <c r="F15" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G15" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H15" s="11">
         <v>1</v>
@@ -1478,10 +1478,10 @@
         <v>16</v>
       </c>
       <c r="F16" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G16" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H16" s="11">
         <v>1</v>
@@ -1519,10 +1519,10 @@
         <v>16</v>
       </c>
       <c r="F17" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G17" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H17" s="11">
         <v>1</v>
@@ -1560,10 +1560,10 @@
         <v>16</v>
       </c>
       <c r="F18" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G18" s="10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H18" s="11">
         <v>1</v>
@@ -1584,7 +1584,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
         <v>33</v>
       </c>
@@ -1625,7 +1625,7 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>33</v>
       </c>
@@ -1666,7 +1666,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>33</v>
       </c>
@@ -1707,7 +1707,7 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
         <v>33</v>
       </c>
@@ -1748,7 +1748,7 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
         <v>33</v>
       </c>
@@ -1789,7 +1789,7 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
         <v>33</v>
       </c>
@@ -1830,7 +1830,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>33</v>
       </c>
@@ -1871,7 +1871,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
         <v>33</v>
       </c>
@@ -1912,7 +1912,7 @@
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>33</v>
       </c>
@@ -1953,7 +1953,7 @@
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
         <v>33</v>
       </c>
@@ -1994,7 +1994,7 @@
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="31" t="s">
         <v>33</v>
       </c>
@@ -2035,7 +2035,7 @@
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
         <v>33</v>
       </c>
@@ -2076,7 +2076,7 @@
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>33</v>
       </c>
@@ -2117,7 +2117,7 @@
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="31" t="s">
         <v>33</v>
       </c>
@@ -2158,7 +2158,7 @@
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
         <v>33</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
         <v>33</v>
       </c>
@@ -2240,7 +2240,7 @@
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
         <v>33</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>35</v>
       </c>
@@ -2322,7 +2322,7 @@
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>35</v>
       </c>
@@ -2363,7 +2363,7 @@
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
         <v>35</v>
       </c>
@@ -2404,7 +2404,7 @@
       <c r="N38" s="7"/>
       <c r="O38" s="7"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>35</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="N39" s="7"/>
       <c r="O39" s="7"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="31" t="s">
         <v>35</v>
       </c>
@@ -2486,7 +2486,7 @@
       <c r="N40" s="7"/>
       <c r="O40" s="7"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>35</v>
       </c>
@@ -2527,7 +2527,7 @@
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>35</v>
       </c>
@@ -2568,7 +2568,7 @@
       <c r="N42" s="7"/>
       <c r="O42" s="7"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
         <v>35</v>
       </c>
@@ -2609,7 +2609,7 @@
       <c r="N43" s="7"/>
       <c r="O43" s="7"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
         <v>35</v>
       </c>
@@ -2650,7 +2650,7 @@
       <c r="N44" s="7"/>
       <c r="O44" s="7"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
         <v>35</v>
       </c>
@@ -2691,7 +2691,7 @@
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="31" t="s">
         <v>35</v>
       </c>
@@ -2732,7 +2732,7 @@
       <c r="N46" s="7"/>
       <c r="O46" s="7"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
         <v>35</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
         <v>35</v>
       </c>
@@ -2814,7 +2814,7 @@
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
         <v>35</v>
       </c>
@@ -2855,7 +2855,7 @@
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
         <v>35</v>
       </c>
@@ -2896,7 +2896,7 @@
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
         <v>35</v>
       </c>
@@ -2937,7 +2937,7 @@
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
         <v>35</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="N52" s="7"/>
       <c r="O52" s="7"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
         <v>37</v>
       </c>
@@ -3019,7 +3019,7 @@
       <c r="N53" s="7"/>
       <c r="O53" s="7"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
         <v>37</v>
       </c>
@@ -3060,7 +3060,7 @@
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="31" t="s">
         <v>37</v>
       </c>
@@ -3101,7 +3101,7 @@
       <c r="N55" s="7"/>
       <c r="O55" s="7"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="31" t="s">
         <v>37</v>
       </c>
@@ -3142,7 +3142,7 @@
       <c r="N56" s="7"/>
       <c r="O56" s="7"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="31" t="s">
         <v>37</v>
       </c>
@@ -3183,7 +3183,7 @@
       <c r="N57" s="7"/>
       <c r="O57" s="7"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="31" t="s">
         <v>37</v>
       </c>
@@ -3224,7 +3224,7 @@
       <c r="N58" s="7"/>
       <c r="O58" s="7"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="31" t="s">
         <v>37</v>
       </c>
@@ -3265,7 +3265,7 @@
       <c r="N59" s="7"/>
       <c r="O59" s="7"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="31" t="s">
         <v>37</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="N60" s="7"/>
       <c r="O60" s="7"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="31" t="s">
         <v>37</v>
       </c>
@@ -3347,7 +3347,7 @@
       <c r="N61" s="7"/>
       <c r="O61" s="7"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="31" t="s">
         <v>37</v>
       </c>
@@ -3388,7 +3388,7 @@
       <c r="N62" s="7"/>
       <c r="O62" s="7"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="31" t="s">
         <v>37</v>
       </c>
@@ -3429,7 +3429,7 @@
       <c r="N63" s="7"/>
       <c r="O63" s="7"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="31" t="s">
         <v>37</v>
       </c>
@@ -3470,7 +3470,7 @@
       <c r="N64" s="7"/>
       <c r="O64" s="7"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="31" t="s">
         <v>37</v>
       </c>
@@ -3511,7 +3511,7 @@
       <c r="N65" s="7"/>
       <c r="O65" s="7"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="31" t="s">
         <v>37</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="N66" s="7"/>
       <c r="O66" s="7"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="31" t="s">
         <v>37</v>
       </c>
@@ -3593,7 +3593,7 @@
       <c r="N67" s="7"/>
       <c r="O67" s="7"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="31" t="s">
         <v>37</v>
       </c>
@@ -3634,7 +3634,7 @@
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="31" t="s">
         <v>37</v>
       </c>
@@ -3675,7 +3675,7 @@
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="31" t="s">
         <v>40</v>
       </c>
@@ -3716,7 +3716,7 @@
       <c r="N70" s="7"/>
       <c r="O70" s="7"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="31" t="s">
         <v>40</v>
       </c>
@@ -3757,7 +3757,7 @@
       <c r="N71" s="7"/>
       <c r="O71" s="7"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="31" t="s">
         <v>40</v>
       </c>
@@ -3798,7 +3798,7 @@
       <c r="N72" s="7"/>
       <c r="O72" s="7"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="31" t="s">
         <v>40</v>
       </c>
@@ -3839,7 +3839,7 @@
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="31" t="s">
         <v>40</v>
       </c>
@@ -3880,7 +3880,7 @@
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="31" t="s">
         <v>40</v>
       </c>
@@ -3921,7 +3921,7 @@
       <c r="N75" s="7"/>
       <c r="O75" s="7"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="31" t="s">
         <v>40</v>
       </c>
@@ -3962,7 +3962,7 @@
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="31" t="s">
         <v>40</v>
       </c>
@@ -4003,7 +4003,7 @@
       <c r="N77" s="7"/>
       <c r="O77" s="7"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="31" t="s">
         <v>40</v>
       </c>
@@ -4044,7 +4044,7 @@
       <c r="N78" s="7"/>
       <c r="O78" s="7"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="31" t="s">
         <v>40</v>
       </c>
@@ -4085,7 +4085,7 @@
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="31" t="s">
         <v>40</v>
       </c>
@@ -4126,7 +4126,7 @@
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="31" t="s">
         <v>40</v>
       </c>
@@ -4167,7 +4167,7 @@
       <c r="N81" s="7"/>
       <c r="O81" s="7"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="31" t="s">
         <v>40</v>
       </c>
@@ -4208,7 +4208,7 @@
       <c r="N82" s="7"/>
       <c r="O82" s="7"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="31" t="s">
         <v>40</v>
       </c>
@@ -4249,7 +4249,7 @@
       <c r="N83" s="7"/>
       <c r="O83" s="7"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="31" t="s">
         <v>40</v>
       </c>
@@ -4290,7 +4290,7 @@
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="31" t="s">
         <v>40</v>
       </c>
@@ -4331,7 +4331,7 @@
       <c r="N85" s="7"/>
       <c r="O85" s="7"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="31" t="s">
         <v>40</v>
       </c>
@@ -4372,7 +4372,7 @@
       <c r="N86" s="7"/>
       <c r="O86" s="7"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="31" t="s">
         <v>42</v>
       </c>
@@ -4413,7 +4413,7 @@
       <c r="N87" s="7"/>
       <c r="O87" s="7"/>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="31" t="s">
         <v>42</v>
       </c>
@@ -4454,7 +4454,7 @@
       <c r="N88" s="7"/>
       <c r="O88" s="7"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="31" t="s">
         <v>42</v>
       </c>
@@ -4495,7 +4495,7 @@
       <c r="N89" s="7"/>
       <c r="O89" s="7"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="31" t="s">
         <v>42</v>
       </c>
@@ -4536,7 +4536,7 @@
       <c r="N90" s="7"/>
       <c r="O90" s="7"/>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="31" t="s">
         <v>42</v>
       </c>
@@ -4577,7 +4577,7 @@
       <c r="N91" s="7"/>
       <c r="O91" s="7"/>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="31" t="s">
         <v>42</v>
       </c>
@@ -4618,7 +4618,7 @@
       <c r="N92" s="7"/>
       <c r="O92" s="7"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="31" t="s">
         <v>42</v>
       </c>
@@ -4659,7 +4659,7 @@
       <c r="N93" s="7"/>
       <c r="O93" s="7"/>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="31" t="s">
         <v>42</v>
       </c>
@@ -4700,7 +4700,7 @@
       <c r="N94" s="7"/>
       <c r="O94" s="7"/>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="31" t="s">
         <v>42</v>
       </c>
@@ -4741,7 +4741,7 @@
       <c r="N95" s="7"/>
       <c r="O95" s="7"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="31" t="s">
         <v>42</v>
       </c>
@@ -4782,7 +4782,7 @@
       <c r="N96" s="7"/>
       <c r="O96" s="7"/>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="31" t="s">
         <v>42</v>
       </c>
@@ -4823,7 +4823,7 @@
       <c r="N97" s="7"/>
       <c r="O97" s="7"/>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="31" t="s">
         <v>42</v>
       </c>
@@ -4864,7 +4864,7 @@
       <c r="N98" s="7"/>
       <c r="O98" s="7"/>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="31" t="s">
         <v>42</v>
       </c>
@@ -4905,7 +4905,7 @@
       <c r="N99" s="7"/>
       <c r="O99" s="7"/>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="31" t="s">
         <v>42</v>
       </c>
@@ -4946,7 +4946,7 @@
       <c r="N100" s="7"/>
       <c r="O100" s="7"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="31" t="s">
         <v>42</v>
       </c>
@@ -4987,7 +4987,7 @@
       <c r="N101" s="7"/>
       <c r="O101" s="7"/>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="31" t="s">
         <v>42</v>
       </c>
@@ -5028,7 +5028,7 @@
       <c r="N102" s="7"/>
       <c r="O102" s="7"/>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="31" t="s">
         <v>42</v>
       </c>
@@ -5069,7 +5069,7 @@
       <c r="N103" s="7"/>
       <c r="O103" s="7"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="31" t="s">
         <v>44</v>
       </c>
@@ -5110,7 +5110,7 @@
       <c r="N104" s="7"/>
       <c r="O104" s="7"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="31" t="s">
         <v>44</v>
       </c>
@@ -5151,7 +5151,7 @@
       <c r="N105" s="7"/>
       <c r="O105" s="7"/>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="31" t="s">
         <v>44</v>
       </c>
@@ -5192,7 +5192,7 @@
       <c r="N106" s="7"/>
       <c r="O106" s="7"/>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="31" t="s">
         <v>44</v>
       </c>
@@ -5233,7 +5233,7 @@
       <c r="N107" s="7"/>
       <c r="O107" s="7"/>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="31" t="s">
         <v>44</v>
       </c>
@@ -5274,7 +5274,7 @@
       <c r="N108" s="7"/>
       <c r="O108" s="7"/>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="31" t="s">
         <v>44</v>
       </c>
@@ -5315,7 +5315,7 @@
       <c r="N109" s="7"/>
       <c r="O109" s="7"/>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="31" t="s">
         <v>44</v>
       </c>
@@ -5356,7 +5356,7 @@
       <c r="N110" s="7"/>
       <c r="O110" s="7"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="31" t="s">
         <v>44</v>
       </c>
@@ -5397,7 +5397,7 @@
       <c r="N111" s="7"/>
       <c r="O111" s="7"/>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="31" t="s">
         <v>44</v>
       </c>
@@ -5438,7 +5438,7 @@
       <c r="N112" s="7"/>
       <c r="O112" s="7"/>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="31" t="s">
         <v>44</v>
       </c>
@@ -5479,7 +5479,7 @@
       <c r="N113" s="7"/>
       <c r="O113" s="7"/>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="31" t="s">
         <v>44</v>
       </c>
@@ -5520,7 +5520,7 @@
       <c r="N114" s="7"/>
       <c r="O114" s="7"/>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="31" t="s">
         <v>44</v>
       </c>
@@ -5561,7 +5561,7 @@
       <c r="N115" s="7"/>
       <c r="O115" s="7"/>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="31" t="s">
         <v>44</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="N116" s="7"/>
       <c r="O116" s="7"/>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="31" t="s">
         <v>44</v>
       </c>
@@ -5643,7 +5643,7 @@
       <c r="N117" s="7"/>
       <c r="O117" s="7"/>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="31" t="s">
         <v>44</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="N118" s="7"/>
       <c r="O118" s="7"/>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="31" t="s">
         <v>44</v>
       </c>
@@ -5725,7 +5725,7 @@
       <c r="N119" s="7"/>
       <c r="O119" s="7"/>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="31" t="s">
         <v>44</v>
       </c>
@@ -5766,7 +5766,7 @@
       <c r="N120" s="7"/>
       <c r="O120" s="7"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="31" t="s">
         <v>46</v>
       </c>
@@ -5807,7 +5807,7 @@
       <c r="N121" s="7"/>
       <c r="O121" s="7"/>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="31" t="s">
         <v>46</v>
       </c>
@@ -5848,7 +5848,7 @@
       <c r="N122" s="7"/>
       <c r="O122" s="7"/>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="31" t="s">
         <v>46</v>
       </c>
@@ -5889,7 +5889,7 @@
       <c r="N123" s="7"/>
       <c r="O123" s="7"/>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="31" t="s">
         <v>46</v>
       </c>
@@ -5930,7 +5930,7 @@
       <c r="N124" s="7"/>
       <c r="O124" s="7"/>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="31" t="s">
         <v>46</v>
       </c>
@@ -5971,7 +5971,7 @@
       <c r="N125" s="7"/>
       <c r="O125" s="7"/>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="31" t="s">
         <v>46</v>
       </c>
@@ -6012,7 +6012,7 @@
       <c r="N126" s="7"/>
       <c r="O126" s="7"/>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="31" t="s">
         <v>46</v>
       </c>
@@ -6053,7 +6053,7 @@
       <c r="N127" s="7"/>
       <c r="O127" s="7"/>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="31" t="s">
         <v>46</v>
       </c>
@@ -6094,7 +6094,7 @@
       <c r="N128" s="7"/>
       <c r="O128" s="7"/>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="31" t="s">
         <v>46</v>
       </c>
@@ -6135,7 +6135,7 @@
       <c r="N129" s="7"/>
       <c r="O129" s="7"/>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="31" t="s">
         <v>46</v>
       </c>
@@ -6176,7 +6176,7 @@
       <c r="N130" s="7"/>
       <c r="O130" s="7"/>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="31" t="s">
         <v>46</v>
       </c>
@@ -6217,7 +6217,7 @@
       <c r="N131" s="7"/>
       <c r="O131" s="7"/>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="31" t="s">
         <v>46</v>
       </c>
@@ -6258,7 +6258,7 @@
       <c r="N132" s="7"/>
       <c r="O132" s="7"/>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="31" t="s">
         <v>46</v>
       </c>
@@ -6299,7 +6299,7 @@
       <c r="N133" s="7"/>
       <c r="O133" s="7"/>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="31" t="s">
         <v>46</v>
       </c>
@@ -6340,7 +6340,7 @@
       <c r="N134" s="7"/>
       <c r="O134" s="7"/>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="31" t="s">
         <v>46</v>
       </c>
@@ -6381,7 +6381,7 @@
       <c r="N135" s="7"/>
       <c r="O135" s="7"/>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="31" t="s">
         <v>46</v>
       </c>
@@ -6422,7 +6422,7 @@
       <c r="N136" s="7"/>
       <c r="O136" s="7"/>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="31" t="s">
         <v>46</v>
       </c>
@@ -6463,7 +6463,7 @@
       <c r="N137" s="7"/>
       <c r="O137" s="7"/>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="31" t="s">
         <v>48</v>
       </c>
@@ -6504,7 +6504,7 @@
       <c r="N138" s="7"/>
       <c r="O138" s="7"/>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="31" t="s">
         <v>48</v>
       </c>
@@ -6545,7 +6545,7 @@
       <c r="N139" s="7"/>
       <c r="O139" s="7"/>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="31" t="s">
         <v>48</v>
       </c>
@@ -6586,7 +6586,7 @@
       <c r="N140" s="7"/>
       <c r="O140" s="7"/>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="31" t="s">
         <v>48</v>
       </c>
@@ -6627,7 +6627,7 @@
       <c r="N141" s="7"/>
       <c r="O141" s="7"/>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="31" t="s">
         <v>48</v>
       </c>
@@ -6668,7 +6668,7 @@
       <c r="N142" s="7"/>
       <c r="O142" s="7"/>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="31" t="s">
         <v>48</v>
       </c>
@@ -6709,7 +6709,7 @@
       <c r="N143" s="7"/>
       <c r="O143" s="7"/>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="31" t="s">
         <v>48</v>
       </c>
@@ -6750,7 +6750,7 @@
       <c r="N144" s="7"/>
       <c r="O144" s="7"/>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="31" t="s">
         <v>48</v>
       </c>
@@ -6791,7 +6791,7 @@
       <c r="N145" s="7"/>
       <c r="O145" s="7"/>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="31" t="s">
         <v>48</v>
       </c>
@@ -6832,7 +6832,7 @@
       <c r="N146" s="7"/>
       <c r="O146" s="7"/>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="31" t="s">
         <v>48</v>
       </c>
@@ -6873,7 +6873,7 @@
       <c r="N147" s="7"/>
       <c r="O147" s="7"/>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="31" t="s">
         <v>48</v>
       </c>
@@ -6914,7 +6914,7 @@
       <c r="N148" s="7"/>
       <c r="O148" s="7"/>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="31" t="s">
         <v>48</v>
       </c>
@@ -6955,7 +6955,7 @@
       <c r="N149" s="7"/>
       <c r="O149" s="7"/>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="31" t="s">
         <v>48</v>
       </c>
@@ -6996,7 +6996,7 @@
       <c r="N150" s="7"/>
       <c r="O150" s="7"/>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="31" t="s">
         <v>48</v>
       </c>
@@ -7037,7 +7037,7 @@
       <c r="N151" s="7"/>
       <c r="O151" s="7"/>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="31" t="s">
         <v>48</v>
       </c>
@@ -7078,7 +7078,7 @@
       <c r="N152" s="7"/>
       <c r="O152" s="7"/>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="31" t="s">
         <v>48</v>
       </c>
@@ -7119,7 +7119,7 @@
       <c r="N153" s="7"/>
       <c r="O153" s="7"/>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="31" t="s">
         <v>48</v>
       </c>
@@ -7160,7 +7160,7 @@
       <c r="N154" s="7"/>
       <c r="O154" s="7"/>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="31" t="s">
         <v>50</v>
       </c>
@@ -7201,7 +7201,7 @@
       <c r="N155" s="7"/>
       <c r="O155" s="7"/>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="31" t="s">
         <v>50</v>
       </c>
@@ -7242,7 +7242,7 @@
       <c r="N156" s="7"/>
       <c r="O156" s="7"/>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="31" t="s">
         <v>50</v>
       </c>
@@ -7283,7 +7283,7 @@
       <c r="N157" s="7"/>
       <c r="O157" s="7"/>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="31" t="s">
         <v>50</v>
       </c>
@@ -7324,7 +7324,7 @@
       <c r="N158" s="7"/>
       <c r="O158" s="7"/>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="31" t="s">
         <v>50</v>
       </c>
@@ -7365,7 +7365,7 @@
       <c r="N159" s="7"/>
       <c r="O159" s="7"/>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="31" t="s">
         <v>50</v>
       </c>
@@ -7406,7 +7406,7 @@
       <c r="N160" s="7"/>
       <c r="O160" s="7"/>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="31" t="s">
         <v>50</v>
       </c>
@@ -7447,7 +7447,7 @@
       <c r="N161" s="7"/>
       <c r="O161" s="7"/>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="31" t="s">
         <v>50</v>
       </c>
@@ -7488,7 +7488,7 @@
       <c r="N162" s="7"/>
       <c r="O162" s="7"/>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="31" t="s">
         <v>50</v>
       </c>
@@ -7529,7 +7529,7 @@
       <c r="N163" s="7"/>
       <c r="O163" s="7"/>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="31" t="s">
         <v>50</v>
       </c>
@@ -7570,7 +7570,7 @@
       <c r="N164" s="7"/>
       <c r="O164" s="7"/>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="31" t="s">
         <v>50</v>
       </c>
@@ -7611,7 +7611,7 @@
       <c r="N165" s="7"/>
       <c r="O165" s="7"/>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="31" t="s">
         <v>50</v>
       </c>
@@ -7652,7 +7652,7 @@
       <c r="N166" s="7"/>
       <c r="O166" s="7"/>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="31" t="s">
         <v>50</v>
       </c>
@@ -7693,7 +7693,7 @@
       <c r="N167" s="7"/>
       <c r="O167" s="7"/>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="31" t="s">
         <v>50</v>
       </c>
@@ -7734,7 +7734,7 @@
       <c r="N168" s="7"/>
       <c r="O168" s="7"/>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="31" t="s">
         <v>50</v>
       </c>
@@ -7775,7 +7775,7 @@
       <c r="N169" s="7"/>
       <c r="O169" s="7"/>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="31" t="s">
         <v>50</v>
       </c>
@@ -7816,7 +7816,7 @@
       <c r="N170" s="7"/>
       <c r="O170" s="7"/>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="31" t="s">
         <v>50</v>
       </c>
@@ -7857,7 +7857,7 @@
       <c r="N171" s="7"/>
       <c r="O171" s="7"/>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="31" t="s">
         <v>52</v>
       </c>
@@ -7898,7 +7898,7 @@
       <c r="N172" s="7"/>
       <c r="O172" s="7"/>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="31" t="s">
         <v>52</v>
       </c>
@@ -7939,7 +7939,7 @@
       <c r="N173" s="7"/>
       <c r="O173" s="7"/>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="31" t="s">
         <v>52</v>
       </c>
@@ -7980,7 +7980,7 @@
       <c r="N174" s="7"/>
       <c r="O174" s="7"/>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="31" t="s">
         <v>52</v>
       </c>
@@ -8021,7 +8021,7 @@
       <c r="N175" s="7"/>
       <c r="O175" s="7"/>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="31" t="s">
         <v>52</v>
       </c>
@@ -8062,7 +8062,7 @@
       <c r="N176" s="7"/>
       <c r="O176" s="7"/>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="31" t="s">
         <v>52</v>
       </c>
@@ -8103,7 +8103,7 @@
       <c r="N177" s="7"/>
       <c r="O177" s="7"/>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="31" t="s">
         <v>52</v>
       </c>
@@ -8144,7 +8144,7 @@
       <c r="N178" s="7"/>
       <c r="O178" s="7"/>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="31" t="s">
         <v>52</v>
       </c>
@@ -8185,7 +8185,7 @@
       <c r="N179" s="7"/>
       <c r="O179" s="7"/>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="31" t="s">
         <v>52</v>
       </c>
@@ -8226,7 +8226,7 @@
       <c r="N180" s="7"/>
       <c r="O180" s="7"/>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="31" t="s">
         <v>52</v>
       </c>
@@ -8267,7 +8267,7 @@
       <c r="N181" s="7"/>
       <c r="O181" s="7"/>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="31" t="s">
         <v>52</v>
       </c>
@@ -8308,7 +8308,7 @@
       <c r="N182" s="7"/>
       <c r="O182" s="7"/>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="31" t="s">
         <v>52</v>
       </c>
@@ -8349,7 +8349,7 @@
       <c r="N183" s="7"/>
       <c r="O183" s="7"/>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="31" t="s">
         <v>52</v>
       </c>
@@ -8390,7 +8390,7 @@
       <c r="N184" s="7"/>
       <c r="O184" s="7"/>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="31" t="s">
         <v>52</v>
       </c>
@@ -8431,7 +8431,7 @@
       <c r="N185" s="7"/>
       <c r="O185" s="7"/>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="31" t="s">
         <v>52</v>
       </c>
@@ -8472,7 +8472,7 @@
       <c r="N186" s="7"/>
       <c r="O186" s="7"/>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="31" t="s">
         <v>52</v>
       </c>
@@ -8513,7 +8513,7 @@
       <c r="N187" s="7"/>
       <c r="O187" s="7"/>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="31" t="s">
         <v>52</v>
       </c>
@@ -8554,7 +8554,7 @@
       <c r="N188" s="7"/>
       <c r="O188" s="7"/>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="31" t="s">
         <v>54</v>
       </c>
@@ -8595,7 +8595,7 @@
       <c r="N189" s="7"/>
       <c r="O189" s="7"/>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="31" t="s">
         <v>54</v>
       </c>
@@ -8636,7 +8636,7 @@
       <c r="N190" s="7"/>
       <c r="O190" s="7"/>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="31" t="s">
         <v>54</v>
       </c>
@@ -8677,7 +8677,7 @@
       <c r="N191" s="7"/>
       <c r="O191" s="7"/>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="31" t="s">
         <v>54</v>
       </c>
@@ -8718,7 +8718,7 @@
       <c r="N192" s="7"/>
       <c r="O192" s="7"/>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="31" t="s">
         <v>54</v>
       </c>
@@ -8759,7 +8759,7 @@
       <c r="N193" s="7"/>
       <c r="O193" s="7"/>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="31" t="s">
         <v>54</v>
       </c>
@@ -8800,7 +8800,7 @@
       <c r="N194" s="7"/>
       <c r="O194" s="7"/>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="31" t="s">
         <v>54</v>
       </c>
@@ -8841,7 +8841,7 @@
       <c r="N195" s="7"/>
       <c r="O195" s="7"/>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="31" t="s">
         <v>54</v>
       </c>
@@ -8882,7 +8882,7 @@
       <c r="N196" s="7"/>
       <c r="O196" s="7"/>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="31" t="s">
         <v>54</v>
       </c>
@@ -8923,7 +8923,7 @@
       <c r="N197" s="7"/>
       <c r="O197" s="7"/>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="31" t="s">
         <v>54</v>
       </c>
@@ -8964,7 +8964,7 @@
       <c r="N198" s="7"/>
       <c r="O198" s="7"/>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="31" t="s">
         <v>54</v>
       </c>
@@ -9005,7 +9005,7 @@
       <c r="N199" s="7"/>
       <c r="O199" s="7"/>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="31" t="s">
         <v>54</v>
       </c>
@@ -9046,7 +9046,7 @@
       <c r="N200" s="7"/>
       <c r="O200" s="7"/>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="31" t="s">
         <v>54</v>
       </c>
@@ -9087,7 +9087,7 @@
       <c r="N201" s="7"/>
       <c r="O201" s="7"/>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="31" t="s">
         <v>54</v>
       </c>
@@ -9128,7 +9128,7 @@
       <c r="N202" s="7"/>
       <c r="O202" s="7"/>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="31" t="s">
         <v>54</v>
       </c>
@@ -9169,7 +9169,7 @@
       <c r="N203" s="7"/>
       <c r="O203" s="7"/>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="31" t="s">
         <v>54</v>
       </c>
@@ -9210,7 +9210,7 @@
       <c r="N204" s="7"/>
       <c r="O204" s="7"/>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="31" t="s">
         <v>54</v>
       </c>
@@ -9251,7 +9251,7 @@
       <c r="N205" s="7"/>
       <c r="O205" s="7"/>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="31" t="s">
         <v>56</v>
       </c>
@@ -9292,7 +9292,7 @@
       <c r="N206" s="7"/>
       <c r="O206" s="7"/>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="31" t="s">
         <v>56</v>
       </c>
@@ -9333,7 +9333,7 @@
       <c r="N207" s="7"/>
       <c r="O207" s="7"/>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="31" t="s">
         <v>56</v>
       </c>
@@ -9374,7 +9374,7 @@
       <c r="N208" s="7"/>
       <c r="O208" s="7"/>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="31" t="s">
         <v>56</v>
       </c>
@@ -9415,7 +9415,7 @@
       <c r="N209" s="7"/>
       <c r="O209" s="7"/>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="31" t="s">
         <v>56</v>
       </c>
@@ -9456,7 +9456,7 @@
       <c r="N210" s="7"/>
       <c r="O210" s="7"/>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="31" t="s">
         <v>56</v>
       </c>
@@ -9497,7 +9497,7 @@
       <c r="N211" s="7"/>
       <c r="O211" s="7"/>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="31" t="s">
         <v>56</v>
       </c>
@@ -9538,7 +9538,7 @@
       <c r="N212" s="7"/>
       <c r="O212" s="7"/>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="31" t="s">
         <v>56</v>
       </c>
@@ -9579,7 +9579,7 @@
       <c r="N213" s="7"/>
       <c r="O213" s="7"/>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="31" t="s">
         <v>56</v>
       </c>
@@ -9620,7 +9620,7 @@
       <c r="N214" s="7"/>
       <c r="O214" s="7"/>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="31" t="s">
         <v>56</v>
       </c>
@@ -9661,7 +9661,7 @@
       <c r="N215" s="7"/>
       <c r="O215" s="7"/>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="31" t="s">
         <v>56</v>
       </c>
@@ -9702,7 +9702,7 @@
       <c r="N216" s="7"/>
       <c r="O216" s="7"/>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="31" t="s">
         <v>56</v>
       </c>
@@ -9743,7 +9743,7 @@
       <c r="N217" s="7"/>
       <c r="O217" s="7"/>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="31" t="s">
         <v>56</v>
       </c>
@@ -9784,7 +9784,7 @@
       <c r="N218" s="7"/>
       <c r="O218" s="7"/>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="31" t="s">
         <v>56</v>
       </c>
@@ -9825,7 +9825,7 @@
       <c r="N219" s="7"/>
       <c r="O219" s="7"/>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="31" t="s">
         <v>56</v>
       </c>
@@ -9866,7 +9866,7 @@
       <c r="N220" s="7"/>
       <c r="O220" s="7"/>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="31" t="s">
         <v>56</v>
       </c>
@@ -9907,7 +9907,7 @@
       <c r="N221" s="7"/>
       <c r="O221" s="7"/>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="31" t="s">
         <v>56</v>
       </c>
@@ -9948,7 +9948,7 @@
       <c r="N222" s="7"/>
       <c r="O222" s="7"/>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="31" t="s">
         <v>58</v>
       </c>
@@ -9989,7 +9989,7 @@
       <c r="N223" s="7"/>
       <c r="O223" s="7"/>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="31" t="s">
         <v>58</v>
       </c>
@@ -10030,7 +10030,7 @@
       <c r="N224" s="7"/>
       <c r="O224" s="7"/>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="31" t="s">
         <v>58</v>
       </c>
@@ -10071,7 +10071,7 @@
       <c r="N225" s="7"/>
       <c r="O225" s="7"/>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="31" t="s">
         <v>58</v>
       </c>
@@ -10112,7 +10112,7 @@
       <c r="N226" s="7"/>
       <c r="O226" s="7"/>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="31" t="s">
         <v>58</v>
       </c>
@@ -10153,7 +10153,7 @@
       <c r="N227" s="7"/>
       <c r="O227" s="7"/>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="31" t="s">
         <v>58</v>
       </c>
@@ -10194,7 +10194,7 @@
       <c r="N228" s="7"/>
       <c r="O228" s="7"/>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="31" t="s">
         <v>58</v>
       </c>
@@ -10235,7 +10235,7 @@
       <c r="N229" s="7"/>
       <c r="O229" s="7"/>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="31" t="s">
         <v>58</v>
       </c>
@@ -10276,7 +10276,7 @@
       <c r="N230" s="7"/>
       <c r="O230" s="7"/>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="31" t="s">
         <v>58</v>
       </c>
@@ -10317,7 +10317,7 @@
       <c r="N231" s="7"/>
       <c r="O231" s="7"/>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="31" t="s">
         <v>58</v>
       </c>
@@ -10358,7 +10358,7 @@
       <c r="N232" s="7"/>
       <c r="O232" s="7"/>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="31" t="s">
         <v>58</v>
       </c>
@@ -10399,7 +10399,7 @@
       <c r="N233" s="7"/>
       <c r="O233" s="7"/>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="31" t="s">
         <v>58</v>
       </c>
@@ -10440,7 +10440,7 @@
       <c r="N234" s="7"/>
       <c r="O234" s="7"/>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="31" t="s">
         <v>58</v>
       </c>
@@ -10481,7 +10481,7 @@
       <c r="N235" s="7"/>
       <c r="O235" s="7"/>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="31" t="s">
         <v>58</v>
       </c>
@@ -10522,7 +10522,7 @@
       <c r="N236" s="7"/>
       <c r="O236" s="7"/>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="31" t="s">
         <v>58</v>
       </c>
@@ -10563,7 +10563,7 @@
       <c r="N237" s="7"/>
       <c r="O237" s="7"/>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="31" t="s">
         <v>58</v>
       </c>
@@ -10604,7 +10604,7 @@
       <c r="N238" s="7"/>
       <c r="O238" s="7"/>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="31" t="s">
         <v>58</v>
       </c>
@@ -10645,7 +10645,7 @@
       <c r="N239" s="7"/>
       <c r="O239" s="7"/>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="31" t="s">
         <v>60</v>
       </c>
@@ -10686,7 +10686,7 @@
       <c r="N240" s="7"/>
       <c r="O240" s="7"/>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="31" t="s">
         <v>60</v>
       </c>
@@ -10727,7 +10727,7 @@
       <c r="N241" s="7"/>
       <c r="O241" s="7"/>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="31" t="s">
         <v>60</v>
       </c>
@@ -10768,7 +10768,7 @@
       <c r="N242" s="7"/>
       <c r="O242" s="7"/>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="31" t="s">
         <v>60</v>
       </c>
@@ -10809,7 +10809,7 @@
       <c r="N243" s="7"/>
       <c r="O243" s="7"/>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="31" t="s">
         <v>60</v>
       </c>
@@ -10850,7 +10850,7 @@
       <c r="N244" s="7"/>
       <c r="O244" s="7"/>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="31" t="s">
         <v>60</v>
       </c>
@@ -10891,7 +10891,7 @@
       <c r="N245" s="7"/>
       <c r="O245" s="7"/>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="31" t="s">
         <v>60</v>
       </c>
@@ -10932,7 +10932,7 @@
       <c r="N246" s="7"/>
       <c r="O246" s="7"/>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="31" t="s">
         <v>60</v>
       </c>
@@ -10973,7 +10973,7 @@
       <c r="N247" s="7"/>
       <c r="O247" s="7"/>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="31" t="s">
         <v>60</v>
       </c>
@@ -11014,7 +11014,7 @@
       <c r="N248" s="7"/>
       <c r="O248" s="7"/>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="31" t="s">
         <v>60</v>
       </c>
@@ -11055,7 +11055,7 @@
       <c r="N249" s="7"/>
       <c r="O249" s="7"/>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="31" t="s">
         <v>60</v>
       </c>
@@ -11096,7 +11096,7 @@
       <c r="N250" s="7"/>
       <c r="O250" s="7"/>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="31" t="s">
         <v>60</v>
       </c>
@@ -11137,7 +11137,7 @@
       <c r="N251" s="7"/>
       <c r="O251" s="7"/>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="31" t="s">
         <v>60</v>
       </c>
@@ -11178,7 +11178,7 @@
       <c r="N252" s="7"/>
       <c r="O252" s="7"/>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="31" t="s">
         <v>60</v>
       </c>
@@ -11219,7 +11219,7 @@
       <c r="N253" s="7"/>
       <c r="O253" s="7"/>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="31" t="s">
         <v>60</v>
       </c>
@@ -11260,7 +11260,7 @@
       <c r="N254" s="7"/>
       <c r="O254" s="7"/>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="31" t="s">
         <v>60</v>
       </c>
@@ -11301,7 +11301,7 @@
       <c r="N255" s="7"/>
       <c r="O255" s="7"/>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="31" t="s">
         <v>60</v>
       </c>
@@ -11342,7 +11342,7 @@
       <c r="N256" s="7"/>
       <c r="O256" s="7"/>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="31" t="s">
         <v>62</v>
       </c>
@@ -11383,7 +11383,7 @@
       <c r="N257" s="7"/>
       <c r="O257" s="7"/>
     </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="31" t="s">
         <v>62</v>
       </c>
@@ -11424,7 +11424,7 @@
       <c r="N258" s="7"/>
       <c r="O258" s="7"/>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="31" t="s">
         <v>62</v>
       </c>
@@ -11465,7 +11465,7 @@
       <c r="N259" s="7"/>
       <c r="O259" s="7"/>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" s="31" t="s">
         <v>62</v>
       </c>
@@ -11506,7 +11506,7 @@
       <c r="N260" s="7"/>
       <c r="O260" s="7"/>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" s="31" t="s">
         <v>62</v>
       </c>
@@ -11547,7 +11547,7 @@
       <c r="N261" s="7"/>
       <c r="O261" s="7"/>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="31" t="s">
         <v>62</v>
       </c>
@@ -11588,7 +11588,7 @@
       <c r="N262" s="7"/>
       <c r="O262" s="7"/>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="31" t="s">
         <v>62</v>
       </c>
@@ -11629,7 +11629,7 @@
       <c r="N263" s="7"/>
       <c r="O263" s="7"/>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" s="31" t="s">
         <v>62</v>
       </c>
@@ -11670,7 +11670,7 @@
       <c r="N264" s="7"/>
       <c r="O264" s="7"/>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="31" t="s">
         <v>62</v>
       </c>
@@ -11711,7 +11711,7 @@
       <c r="N265" s="7"/>
       <c r="O265" s="7"/>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" s="31" t="s">
         <v>62</v>
       </c>
@@ -11752,7 +11752,7 @@
       <c r="N266" s="7"/>
       <c r="O266" s="7"/>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" s="31" t="s">
         <v>62</v>
       </c>
@@ -11793,7 +11793,7 @@
       <c r="N267" s="7"/>
       <c r="O267" s="7"/>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="31" t="s">
         <v>62</v>
       </c>
@@ -11834,7 +11834,7 @@
       <c r="N268" s="7"/>
       <c r="O268" s="7"/>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" s="31" t="s">
         <v>62</v>
       </c>
@@ -11875,7 +11875,7 @@
       <c r="N269" s="7"/>
       <c r="O269" s="7"/>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="31" t="s">
         <v>62</v>
       </c>
@@ -11916,7 +11916,7 @@
       <c r="N270" s="7"/>
       <c r="O270" s="7"/>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="31" t="s">
         <v>62</v>
       </c>
@@ -11957,7 +11957,7 @@
       <c r="N271" s="7"/>
       <c r="O271" s="7"/>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="31" t="s">
         <v>62</v>
       </c>
@@ -11998,7 +11998,7 @@
       <c r="N272" s="7"/>
       <c r="O272" s="7"/>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="31" t="s">
         <v>62</v>
       </c>
@@ -12039,7 +12039,7 @@
       <c r="N273" s="7"/>
       <c r="O273" s="7"/>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" s="31" t="s">
         <v>64</v>
       </c>
@@ -12059,10 +12059,10 @@
         <v>284</v>
       </c>
       <c r="G274" s="10">
-        <v>104.66666666666667</v>
+        <v>314</v>
       </c>
       <c r="H274" s="11">
-        <v>2.7133757961783438</v>
+        <v>0.90445859872611467</v>
       </c>
       <c r="I274" s="11">
         <v>0.90039999999999998</v>
@@ -12074,13 +12074,13 @@
         <v>0.06</v>
       </c>
       <c r="L274" s="15">
-        <v>3.0135226523526697</v>
+        <v>1.0045075507842234</v>
       </c>
       <c r="M274" s="7"/>
       <c r="N274" s="7"/>
       <c r="O274" s="7"/>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" s="31" t="s">
         <v>64</v>
       </c>
@@ -12100,10 +12100,10 @@
         <v>69</v>
       </c>
       <c r="G275" s="10">
-        <v>23.333333333333332</v>
+        <v>70</v>
       </c>
       <c r="H275" s="11">
-        <v>2.9571428571428573</v>
+        <v>0.98571428571428577</v>
       </c>
       <c r="I275" s="11">
         <v>0.90039999999999998</v>
@@ -12115,13 +12115,13 @@
         <v>0.06</v>
       </c>
       <c r="L275" s="15">
-        <v>3.284254616995621</v>
+        <v>1.0947515389985405</v>
       </c>
       <c r="M275" s="7"/>
       <c r="N275" s="7"/>
       <c r="O275" s="7"/>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" s="31" t="s">
         <v>64</v>
       </c>
@@ -12141,10 +12141,10 @@
         <v>47</v>
       </c>
       <c r="G276" s="10">
-        <v>19.666666666666668</v>
+        <v>59</v>
       </c>
       <c r="H276" s="11">
-        <v>2.3898305084745761</v>
+        <v>0.79661016949152541</v>
       </c>
       <c r="I276" s="11">
         <v>0.90039999999999998</v>
@@ -12153,16 +12153,16 @@
         <v>0.06</v>
       </c>
       <c r="K276" s="14">
-        <v>0.06</v>
+        <v>5.3083751854166507E-2</v>
       </c>
       <c r="L276" s="15">
-        <v>2.6541875927083254</v>
+        <v>0.88472919756944179</v>
       </c>
       <c r="M276" s="7"/>
       <c r="N276" s="7"/>
       <c r="O276" s="7"/>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" s="31" t="s">
         <v>64</v>
       </c>
@@ -12182,10 +12182,10 @@
         <v>8</v>
       </c>
       <c r="G277" s="10">
-        <v>3.3333333333333335</v>
+        <v>10</v>
       </c>
       <c r="H277" s="11">
-        <v>2.4</v>
+        <v>0.8</v>
       </c>
       <c r="I277" s="11">
         <v>0.90039999999999998</v>
@@ -12194,16 +12194,16 @@
         <v>0.06</v>
       </c>
       <c r="K277" s="14">
-        <v>0.06</v>
+        <v>5.3309640159928923E-2</v>
       </c>
       <c r="L277" s="15">
-        <v>2.6654820079964461</v>
+        <v>0.88849400266548206</v>
       </c>
       <c r="M277" s="7"/>
       <c r="N277" s="7"/>
       <c r="O277" s="7"/>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" s="31" t="s">
         <v>64</v>
       </c>
@@ -12223,10 +12223,10 @@
         <v>42</v>
       </c>
       <c r="G278" s="10">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="H278" s="11">
-        <v>2.8</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="I278" s="11">
         <v>0.90039999999999998</v>
@@ -12238,13 +12238,13 @@
         <v>0.06</v>
       </c>
       <c r="L278" s="15">
-        <v>3.1097290093291869</v>
+        <v>1.0365763364430625</v>
       </c>
       <c r="M278" s="7"/>
       <c r="N278" s="7"/>
       <c r="O278" s="7"/>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="31" t="s">
         <v>64</v>
       </c>
@@ -12285,7 +12285,7 @@
       <c r="N279" s="7"/>
       <c r="O279" s="7"/>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" s="31" t="s">
         <v>64</v>
       </c>
@@ -12305,10 +12305,10 @@
         <v>74</v>
       </c>
       <c r="G280" s="10">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="H280" s="11">
-        <v>2.6428571428571428</v>
+        <v>0.88095238095238093</v>
       </c>
       <c r="I280" s="11">
         <v>0.90039999999999998</v>
@@ -12317,16 +12317,16 @@
         <v>0.06</v>
       </c>
       <c r="K280" s="14">
-        <v>0.06</v>
+        <v>5.8704068033255057E-2</v>
       </c>
       <c r="L280" s="15">
-        <v>2.9352034016627528</v>
+        <v>0.97840113388758432</v>
       </c>
       <c r="M280" s="7"/>
       <c r="N280" s="7"/>
       <c r="O280" s="7"/>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="31" t="s">
         <v>64</v>
       </c>
@@ -12367,7 +12367,7 @@
       <c r="N281" s="7"/>
       <c r="O281" s="7"/>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="31" t="s">
         <v>64</v>
       </c>
@@ -12387,10 +12387,10 @@
         <v>19</v>
       </c>
       <c r="G282" s="10">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H282" s="11">
-        <v>2.7142857142857144</v>
+        <v>0.90476190476190477</v>
       </c>
       <c r="I282" s="11">
         <v>0.90039999999999998</v>
@@ -12402,13 +12402,13 @@
         <v>0.06</v>
       </c>
       <c r="L282" s="15">
-        <v>3.0145332233293143</v>
+        <v>1.004844407776438</v>
       </c>
       <c r="M282" s="7"/>
       <c r="N282" s="7"/>
       <c r="O282" s="7"/>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" s="31" t="s">
         <v>64</v>
       </c>
@@ -12428,10 +12428,10 @@
         <v>7</v>
       </c>
       <c r="G283" s="10">
-        <v>2.3333333333333335</v>
+        <v>7</v>
       </c>
       <c r="H283" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I283" s="11">
         <v>0.90039999999999998</v>
@@ -12443,13 +12443,13 @@
         <v>0.06</v>
       </c>
       <c r="L283" s="15">
-        <v>3.3318525099955578</v>
+        <v>1.1106175033318526</v>
       </c>
       <c r="M283" s="7"/>
       <c r="N283" s="7"/>
       <c r="O283" s="7"/>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="31" t="s">
         <v>64</v>
       </c>
@@ -12469,10 +12469,10 @@
         <v>16</v>
       </c>
       <c r="G284" s="10">
-        <v>5.333333333333333</v>
+        <v>16</v>
       </c>
       <c r="H284" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I284" s="11">
         <v>0.90039999999999998</v>
@@ -12484,13 +12484,13 @@
         <v>0.06</v>
       </c>
       <c r="L284" s="15">
-        <v>3.3318525099955578</v>
+        <v>1.1106175033318526</v>
       </c>
       <c r="M284" s="7"/>
       <c r="N284" s="7"/>
       <c r="O284" s="7"/>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="31" t="s">
         <v>64</v>
       </c>
@@ -12531,7 +12531,7 @@
       <c r="N285" s="7"/>
       <c r="O285" s="7"/>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="31" t="s">
         <v>64</v>
       </c>
@@ -12572,7 +12572,7 @@
       <c r="N286" s="7"/>
       <c r="O286" s="7"/>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="31" t="s">
         <v>64</v>
       </c>
@@ -12613,7 +12613,7 @@
       <c r="N287" s="7"/>
       <c r="O287" s="7"/>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="31" t="s">
         <v>64</v>
       </c>
@@ -12654,7 +12654,7 @@
       <c r="N288" s="7"/>
       <c r="O288" s="7"/>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="31" t="s">
         <v>64</v>
       </c>
@@ -12674,10 +12674,10 @@
         <v>2</v>
       </c>
       <c r="G289" s="10">
-        <v>0.66666666666666663</v>
+        <v>2</v>
       </c>
       <c r="H289" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I289" s="11">
         <v>0.90039999999999998</v>
@@ -12689,13 +12689,13 @@
         <v>0.06</v>
       </c>
       <c r="L289" s="15">
-        <v>3.3318525099955578</v>
+        <v>1.1106175033318526</v>
       </c>
       <c r="M289" s="7"/>
       <c r="N289" s="7"/>
       <c r="O289" s="7"/>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="31" t="s">
         <v>64</v>
       </c>
@@ -12715,10 +12715,10 @@
         <v>1853</v>
       </c>
       <c r="G290" s="10">
-        <v>689.66666666666663</v>
+        <v>2069</v>
       </c>
       <c r="H290" s="11">
-        <v>2.6868052199130017</v>
+        <v>0.89560173997100045</v>
       </c>
       <c r="I290" s="11">
         <v>0.90039999999999998</v>
@@ -12727,16 +12727,16 @@
         <v>0.06</v>
       </c>
       <c r="K290" s="14">
-        <v>0.06</v>
+        <v>5.9680258105575333E-2</v>
       </c>
       <c r="L290" s="15">
-        <v>2.9840129052787669</v>
+        <v>0.99467096842625558</v>
       </c>
       <c r="M290" s="7"/>
       <c r="N290" s="7"/>
       <c r="O290" s="7"/>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="31" t="s">
         <v>66</v>
       </c>
@@ -12753,13 +12753,13 @@
         <v>16</v>
       </c>
       <c r="F291" s="10">
-        <v>7380</v>
+        <v>2460</v>
       </c>
       <c r="G291" s="10">
         <v>9956</v>
       </c>
       <c r="H291" s="11">
-        <v>0.74126155082362399</v>
+        <v>0.24708718360787466</v>
       </c>
       <c r="I291" s="11">
         <v>0.2591</v>
@@ -12768,16 +12768,16 @@
         <v>0.06</v>
       </c>
       <c r="K291" s="14">
-        <v>0.06</v>
+        <v>5.7218182232622455E-2</v>
       </c>
       <c r="L291" s="15">
-        <v>2.8609091116311229</v>
+        <v>0.95363637054370765</v>
       </c>
       <c r="M291" s="7"/>
       <c r="N291" s="7"/>
       <c r="O291" s="7"/>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="31" t="s">
         <v>66</v>
       </c>
@@ -12794,13 +12794,13 @@
         <v>16</v>
       </c>
       <c r="F292" s="10">
-        <v>2220</v>
+        <v>740</v>
       </c>
       <c r="G292" s="10">
         <v>2773</v>
       </c>
       <c r="H292" s="11">
-        <v>0.80057699242697444</v>
+        <v>0.26685899747565811</v>
       </c>
       <c r="I292" s="11">
         <v>0.2591</v>
@@ -12812,13 +12812,13 @@
         <v>0.06</v>
       </c>
       <c r="L292" s="15">
-        <v>3.0898378711963508</v>
+        <v>1.0299459570654501</v>
       </c>
       <c r="M292" s="7"/>
       <c r="N292" s="7"/>
       <c r="O292" s="7"/>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="31" t="s">
         <v>66</v>
       </c>
@@ -12835,13 +12835,13 @@
         <v>16</v>
       </c>
       <c r="F293" s="10">
-        <v>1119</v>
+        <v>373</v>
       </c>
       <c r="G293" s="10">
         <v>1746</v>
       </c>
       <c r="H293" s="11">
-        <v>0.64089347079037806</v>
+        <v>0.21363115693012599</v>
       </c>
       <c r="I293" s="11">
         <v>0.2591</v>
@@ -12850,16 +12850,16 @@
         <v>0.06</v>
       </c>
       <c r="K293" s="14">
-        <v>0.06</v>
+        <v>4.9470742631445616E-2</v>
       </c>
       <c r="L293" s="15">
-        <v>2.4735371315722814</v>
+        <v>0.82451237719076031</v>
       </c>
       <c r="M293" s="7"/>
       <c r="N293" s="7"/>
       <c r="O293" s="7"/>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="31" t="s">
         <v>66</v>
       </c>
@@ -12876,7 +12876,7 @@
         <v>16</v>
       </c>
       <c r="F294" s="10">
-        <v>252</v>
+        <v>84</v>
       </c>
       <c r="G294" s="10">
         <v>0</v>
@@ -12900,7 +12900,7 @@
       <c r="N294" s="7"/>
       <c r="O294" s="7"/>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="31" t="s">
         <v>66</v>
       </c>
@@ -12917,13 +12917,13 @@
         <v>16</v>
       </c>
       <c r="F295" s="10">
-        <v>1029</v>
+        <v>343</v>
       </c>
       <c r="G295" s="10">
         <v>1579</v>
       </c>
       <c r="H295" s="11">
-        <v>0.65167827739075368</v>
+        <v>0.21722609246358454</v>
       </c>
       <c r="I295" s="11">
         <v>0.2591</v>
@@ -12932,16 +12932,16 @@
         <v>0.06</v>
       </c>
       <c r="K295" s="14">
-        <v>0.06</v>
+        <v>5.0303224808240336E-2</v>
       </c>
       <c r="L295" s="15">
-        <v>2.5151612404120174</v>
+        <v>0.83838708013733898</v>
       </c>
       <c r="M295" s="7"/>
       <c r="N295" s="7"/>
       <c r="O295" s="7"/>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="31" t="s">
         <v>66</v>
       </c>
@@ -12958,7 +12958,7 @@
         <v>16</v>
       </c>
       <c r="F296" s="10">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G296" s="10">
         <v>0</v>
@@ -12982,7 +12982,7 @@
       <c r="N296" s="7"/>
       <c r="O296" s="7"/>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" s="31" t="s">
         <v>66</v>
       </c>
@@ -12999,13 +12999,13 @@
         <v>16</v>
       </c>
       <c r="F297" s="10">
-        <v>1161</v>
+        <v>387</v>
       </c>
       <c r="G297" s="10">
         <v>1891</v>
       </c>
       <c r="H297" s="11">
-        <v>0.61396086726599686</v>
+        <v>0.20465362242199894</v>
       </c>
       <c r="I297" s="11">
         <v>0.2591</v>
@@ -13014,16 +13014,16 @@
         <v>0.06</v>
       </c>
       <c r="K297" s="14">
-        <v>0.06</v>
+        <v>4.7391807585179226E-2</v>
       </c>
       <c r="L297" s="15">
-        <v>2.3695903792589612</v>
+        <v>0.78986345975298711</v>
       </c>
       <c r="M297" s="7"/>
       <c r="N297" s="7"/>
       <c r="O297" s="7"/>
     </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="31" t="s">
         <v>66</v>
       </c>
@@ -13040,7 +13040,7 @@
         <v>16</v>
       </c>
       <c r="F298" s="10">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G298" s="10">
         <v>0</v>
@@ -13064,7 +13064,7 @@
       <c r="N298" s="7"/>
       <c r="O298" s="7"/>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" s="31" t="s">
         <v>66</v>
       </c>
@@ -13081,13 +13081,13 @@
         <v>16</v>
       </c>
       <c r="F299" s="10">
-        <v>576</v>
+        <v>192</v>
       </c>
       <c r="G299" s="10">
         <v>1062</v>
       </c>
       <c r="H299" s="11">
-        <v>0.5423728813559322</v>
+        <v>0.1807909604519774</v>
       </c>
       <c r="I299" s="11">
         <v>0.2591</v>
@@ -13096,16 +13096,16 @@
         <v>0.06</v>
       </c>
       <c r="K299" s="14">
-        <v>0.06</v>
+        <v>4.1865911335849645E-2</v>
       </c>
       <c r="L299" s="15">
-        <v>2.0932955667924826</v>
+        <v>0.69776518893082751</v>
       </c>
       <c r="M299" s="7"/>
       <c r="N299" s="7"/>
       <c r="O299" s="7"/>
     </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="31" t="s">
         <v>66</v>
       </c>
@@ -13122,7 +13122,7 @@
         <v>16</v>
       </c>
       <c r="F300" s="10">
-        <v>273</v>
+        <v>91</v>
       </c>
       <c r="G300" s="10">
         <v>0</v>
@@ -13146,7 +13146,7 @@
       <c r="N300" s="7"/>
       <c r="O300" s="7"/>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="31" t="s">
         <v>66</v>
       </c>
@@ -13163,13 +13163,13 @@
         <v>16</v>
       </c>
       <c r="F301" s="10">
-        <v>612</v>
+        <v>204</v>
       </c>
       <c r="G301" s="10">
         <v>905</v>
       </c>
       <c r="H301" s="11">
-        <v>0.67624309392265192</v>
+        <v>0.22541436464088399</v>
       </c>
       <c r="I301" s="11">
         <v>0.2591</v>
@@ -13178,16 +13178,16 @@
         <v>0.06</v>
       </c>
       <c r="K301" s="14">
-        <v>0.06</v>
+        <v>5.219938972772304E-2</v>
       </c>
       <c r="L301" s="15">
-        <v>2.6099694863861518</v>
+        <v>0.869989828795384</v>
       </c>
       <c r="M301" s="7"/>
       <c r="N301" s="7"/>
       <c r="O301" s="7"/>
     </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="31" t="s">
         <v>66</v>
       </c>
@@ -13204,7 +13204,7 @@
         <v>16</v>
       </c>
       <c r="F302" s="10">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G302" s="10">
         <v>0</v>
@@ -13228,7 +13228,7 @@
       <c r="N302" s="7"/>
       <c r="O302" s="7"/>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="31" t="s">
         <v>66</v>
       </c>
@@ -13269,7 +13269,7 @@
       <c r="N303" s="7"/>
       <c r="O303" s="7"/>
     </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="31" t="s">
         <v>66</v>
       </c>
@@ -13286,7 +13286,7 @@
         <v>16</v>
       </c>
       <c r="F304" s="10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G304" s="10">
         <v>0</v>
@@ -13310,7 +13310,7 @@
       <c r="N304" s="7"/>
       <c r="O304" s="7"/>
     </row>
-    <row r="305" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="31" t="s">
         <v>66</v>
       </c>
@@ -13327,7 +13327,7 @@
         <v>16</v>
       </c>
       <c r="F305" s="10">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G305" s="10">
         <v>0</v>
@@ -13351,7 +13351,7 @@
       <c r="N305" s="7"/>
       <c r="O305" s="7"/>
     </row>
-    <row r="306" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="31" t="s">
         <v>66</v>
       </c>
@@ -13368,7 +13368,7 @@
         <v>16</v>
       </c>
       <c r="F306" s="10">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="G306" s="10">
         <v>0</v>
@@ -13392,7 +13392,7 @@
       <c r="N306" s="7"/>
       <c r="O306" s="7"/>
     </row>
-    <row r="307" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="31" t="s">
         <v>66</v>
       </c>
@@ -13409,7 +13409,7 @@
         <v>16</v>
       </c>
       <c r="F307" s="10">
-        <v>50427</v>
+        <v>16809</v>
       </c>
       <c r="G307" s="10">
         <v>0</v>
@@ -13433,7 +13433,7 @@
       <c r="N307" s="7"/>
       <c r="O307" s="7"/>
     </row>
-    <row r="308" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="31" t="s">
         <v>68</v>
       </c>
@@ -13450,13 +13450,13 @@
         <v>16</v>
       </c>
       <c r="F308" s="10">
-        <v>32976</v>
+        <v>10992</v>
       </c>
       <c r="G308" s="10">
         <v>16542</v>
       </c>
       <c r="H308" s="11">
-        <v>1.9934711643090315</v>
+        <v>0.66449038810301053</v>
       </c>
       <c r="I308" s="11">
         <v>0.71</v>
@@ -13465,16 +13465,16 @@
         <v>0.06</v>
       </c>
       <c r="K308" s="14">
-        <v>0.06</v>
+        <v>5.6154117304479764E-2</v>
       </c>
       <c r="L308" s="15">
-        <v>2.8077058652239884</v>
+        <v>0.93590195507466278</v>
       </c>
       <c r="M308" s="7"/>
       <c r="N308" s="7"/>
       <c r="O308" s="7"/>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" s="31" t="s">
         <v>68</v>
       </c>
@@ -13491,13 +13491,13 @@
         <v>16</v>
       </c>
       <c r="F309" s="10">
-        <v>8703</v>
+        <v>2901</v>
       </c>
       <c r="G309" s="10">
         <v>4868</v>
       </c>
       <c r="H309" s="11">
-        <v>1.7877978635990139</v>
+        <v>0.59593262119967128</v>
       </c>
       <c r="I309" s="11">
         <v>0.71</v>
@@ -13506,16 +13506,16 @@
         <v>0.06</v>
       </c>
       <c r="K309" s="14">
-        <v>0.06</v>
+        <v>5.036050319997222E-2</v>
       </c>
       <c r="L309" s="15">
-        <v>2.5180251599986114</v>
+        <v>0.83934171999953699</v>
       </c>
       <c r="M309" s="7"/>
       <c r="N309" s="7"/>
       <c r="O309" s="7"/>
     </row>
-    <row r="310" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" s="31" t="s">
         <v>68</v>
       </c>
@@ -13532,13 +13532,13 @@
         <v>16</v>
       </c>
       <c r="F310" s="10">
-        <v>5913</v>
+        <v>1971</v>
       </c>
       <c r="G310" s="10">
         <v>3100</v>
       </c>
       <c r="H310" s="11">
-        <v>1.9074193548387097</v>
+        <v>0.63580645161290328</v>
       </c>
       <c r="I310" s="11">
         <v>0.71</v>
@@ -13547,16 +13547,16 @@
         <v>0.06</v>
       </c>
       <c r="K310" s="14">
-        <v>0.06</v>
+        <v>5.3730122671512955E-2</v>
       </c>
       <c r="L310" s="15">
-        <v>2.6865061335756475</v>
+        <v>0.89550204452521598</v>
       </c>
       <c r="M310" s="7"/>
       <c r="N310" s="7"/>
       <c r="O310" s="7"/>
     </row>
-    <row r="311" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="31" t="s">
         <v>68</v>
       </c>
@@ -13573,7 +13573,7 @@
         <v>16</v>
       </c>
       <c r="F311" s="10">
-        <v>939</v>
+        <v>313</v>
       </c>
       <c r="G311" s="10">
         <v>0</v>
@@ -13597,7 +13597,7 @@
       <c r="N311" s="7"/>
       <c r="O311" s="7"/>
     </row>
-    <row r="312" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" s="31" t="s">
         <v>68</v>
       </c>
@@ -13614,13 +13614,13 @@
         <v>16</v>
       </c>
       <c r="F312" s="10">
-        <v>4746</v>
+        <v>1582</v>
       </c>
       <c r="G312" s="10">
         <v>2564</v>
       </c>
       <c r="H312" s="11">
-        <v>1.8510140405616224</v>
+        <v>0.61700468018720744</v>
       </c>
       <c r="I312" s="11">
         <v>0.71</v>
@@ -13629,16 +13629,16 @@
         <v>0.06</v>
       </c>
       <c r="K312" s="14">
-        <v>0.06</v>
+        <v>5.214124057920063E-2</v>
       </c>
       <c r="L312" s="15">
-        <v>2.6070620289600317</v>
+        <v>0.86902067632001057</v>
       </c>
       <c r="M312" s="7"/>
       <c r="N312" s="7"/>
       <c r="O312" s="7"/>
     </row>
-    <row r="313" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="31" t="s">
         <v>68</v>
       </c>
@@ -13655,7 +13655,7 @@
         <v>16</v>
       </c>
       <c r="F313" s="10">
-        <v>171</v>
+        <v>57</v>
       </c>
       <c r="G313" s="10">
         <v>0</v>
@@ -13679,7 +13679,7 @@
       <c r="N313" s="7"/>
       <c r="O313" s="7"/>
     </row>
-    <row r="314" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="31" t="s">
         <v>68</v>
       </c>
@@ -13696,13 +13696,13 @@
         <v>16</v>
       </c>
       <c r="F314" s="10">
-        <v>5403</v>
+        <v>1801</v>
       </c>
       <c r="G314" s="10">
         <v>2982</v>
       </c>
       <c r="H314" s="11">
-        <v>1.811871227364185</v>
+        <v>0.60395707578806168</v>
       </c>
       <c r="I314" s="11">
         <v>0.71</v>
@@ -13711,16 +13711,16 @@
         <v>0.06</v>
       </c>
       <c r="K314" s="14">
-        <v>0.06</v>
+        <v>5.1038626122934791E-2</v>
       </c>
       <c r="L314" s="15">
-        <v>2.5519313061467397</v>
+        <v>0.8506437687155799</v>
       </c>
       <c r="M314" s="7"/>
       <c r="N314" s="7"/>
       <c r="O314" s="7"/>
     </row>
-    <row r="315" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" s="31" t="s">
         <v>68</v>
       </c>
@@ -13737,7 +13737,7 @@
         <v>16</v>
       </c>
       <c r="F315" s="10">
-        <v>189</v>
+        <v>63</v>
       </c>
       <c r="G315" s="10">
         <v>0</v>
@@ -13761,7 +13761,7 @@
       <c r="N315" s="7"/>
       <c r="O315" s="7"/>
     </row>
-    <row r="316" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="31" t="s">
         <v>68</v>
       </c>
@@ -13778,13 +13778,13 @@
         <v>16</v>
       </c>
       <c r="F316" s="10">
-        <v>2568</v>
+        <v>856</v>
       </c>
       <c r="G316" s="10">
         <v>1419</v>
       </c>
       <c r="H316" s="11">
-        <v>1.8097251585623679</v>
+        <v>0.60324171952078931</v>
       </c>
       <c r="I316" s="11">
         <v>0.71</v>
@@ -13793,16 +13793,16 @@
         <v>0.06</v>
       </c>
       <c r="K316" s="14">
-        <v>0.06</v>
+        <v>5.0978173480630079E-2</v>
       </c>
       <c r="L316" s="15">
-        <v>2.5489086740315043</v>
+        <v>0.84963622467716804</v>
       </c>
       <c r="M316" s="7"/>
       <c r="N316" s="7"/>
       <c r="O316" s="7"/>
     </row>
-    <row r="317" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" s="31" t="s">
         <v>68</v>
       </c>
@@ -13819,7 +13819,7 @@
         <v>16</v>
       </c>
       <c r="F317" s="10">
-        <v>576</v>
+        <v>192</v>
       </c>
       <c r="G317" s="10">
         <v>0</v>
@@ -13843,7 +13843,7 @@
       <c r="N317" s="7"/>
       <c r="O317" s="7"/>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="31" t="s">
         <v>68</v>
       </c>
@@ -13860,13 +13860,13 @@
         <v>16</v>
       </c>
       <c r="F318" s="10">
-        <v>2934</v>
+        <v>978</v>
       </c>
       <c r="G318" s="10">
         <v>1608</v>
       </c>
       <c r="H318" s="11">
-        <v>1.8246268656716418</v>
+        <v>0.60820895522388063</v>
       </c>
       <c r="I318" s="11">
         <v>0.71</v>
@@ -13875,16 +13875,16 @@
         <v>0.06</v>
       </c>
       <c r="K318" s="14">
-        <v>0.06</v>
+        <v>5.1397939878074422E-2</v>
       </c>
       <c r="L318" s="15">
-        <v>2.5698969939037211</v>
+        <v>0.85663233130124039</v>
       </c>
       <c r="M318" s="7"/>
       <c r="N318" s="7"/>
       <c r="O318" s="7"/>
     </row>
-    <row r="319" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="31" t="s">
         <v>68</v>
       </c>
@@ -13901,7 +13901,7 @@
         <v>16</v>
       </c>
       <c r="F319" s="10">
-        <v>189</v>
+        <v>63</v>
       </c>
       <c r="G319" s="10">
         <v>0</v>
@@ -13925,7 +13925,7 @@
       <c r="N319" s="7"/>
       <c r="O319" s="7"/>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="31" t="s">
         <v>68</v>
       </c>
@@ -13942,7 +13942,7 @@
         <v>16</v>
       </c>
       <c r="F320" s="10">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="G320" s="10">
         <v>0</v>
@@ -13966,7 +13966,7 @@
       <c r="N320" s="7"/>
       <c r="O320" s="7"/>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" s="31" t="s">
         <v>68</v>
       </c>
@@ -13983,7 +13983,7 @@
         <v>16</v>
       </c>
       <c r="F321" s="10">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="G321" s="10">
         <v>0</v>
@@ -14007,7 +14007,7 @@
       <c r="N321" s="7"/>
       <c r="O321" s="7"/>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" s="31" t="s">
         <v>68</v>
       </c>
@@ -14024,7 +14024,7 @@
         <v>16</v>
       </c>
       <c r="F322" s="10">
-        <v>156</v>
+        <v>52</v>
       </c>
       <c r="G322" s="10">
         <v>0</v>
@@ -14048,7 +14048,7 @@
       <c r="N322" s="7"/>
       <c r="O322" s="7"/>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" s="31" t="s">
         <v>68</v>
       </c>
@@ -14065,7 +14065,7 @@
         <v>16</v>
       </c>
       <c r="F323" s="10">
-        <v>297</v>
+        <v>99</v>
       </c>
       <c r="G323" s="10">
         <v>0</v>
@@ -14089,7 +14089,7 @@
       <c r="N323" s="7"/>
       <c r="O323" s="7"/>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="31" t="s">
         <v>68</v>
       </c>
@@ -14106,7 +14106,7 @@
         <v>16</v>
       </c>
       <c r="F324" s="10">
-        <v>269430</v>
+        <v>89810</v>
       </c>
       <c r="G324" s="10">
         <v>0</v>
@@ -14130,7 +14130,7 @@
       <c r="N324" s="7"/>
       <c r="O324" s="7"/>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" s="31" t="s">
         <v>70</v>
       </c>
@@ -14147,13 +14147,13 @@
         <v>16</v>
       </c>
       <c r="F325" s="10">
-        <v>66216</v>
+        <v>22072</v>
       </c>
       <c r="G325" s="10">
         <v>37391</v>
       </c>
       <c r="H325" s="11">
-        <v>1.7709074376186782</v>
+        <v>0.59030247920622614</v>
       </c>
       <c r="I325" s="11">
         <v>0.63500000000000001</v>
@@ -14162,16 +14162,16 @@
         <v>0.06</v>
       </c>
       <c r="K325" s="14">
-        <v>0.06</v>
+        <v>5.5776612208462306E-2</v>
       </c>
       <c r="L325" s="15">
-        <v>2.7888306104231151</v>
+        <v>0.92961020347437184</v>
       </c>
       <c r="M325" s="7"/>
       <c r="N325" s="7"/>
       <c r="O325" s="7"/>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" s="31" t="s">
         <v>70</v>
       </c>
@@ -14188,13 +14188,13 @@
         <v>16</v>
       </c>
       <c r="F326" s="10">
-        <v>17430</v>
+        <v>5810</v>
       </c>
       <c r="G326" s="10">
         <v>11065</v>
       </c>
       <c r="H326" s="11">
-        <v>1.5752372345232715</v>
+        <v>0.5250790781744239</v>
       </c>
       <c r="I326" s="11">
         <v>0.63500000000000001</v>
@@ -14203,16 +14203,16 @@
         <v>0.06</v>
       </c>
       <c r="K326" s="14">
-        <v>0.06</v>
+        <v>4.9613771166087298E-2</v>
       </c>
       <c r="L326" s="15">
-        <v>2.4806885583043643</v>
+        <v>0.82689618610145499</v>
       </c>
       <c r="M326" s="7"/>
       <c r="N326" s="7"/>
       <c r="O326" s="7"/>
     </row>
-    <row r="327" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" s="31" t="s">
         <v>70</v>
       </c>
@@ -14229,13 +14229,13 @@
         <v>16</v>
       </c>
       <c r="F327" s="10">
-        <v>11325</v>
+        <v>3775</v>
       </c>
       <c r="G327" s="10">
         <v>6986</v>
       </c>
       <c r="H327" s="11">
-        <v>1.6210993415402233</v>
+        <v>0.54036644718007443</v>
       </c>
       <c r="I327" s="11">
         <v>0.63500000000000001</v>
@@ -14244,16 +14244,16 @@
         <v>0.06</v>
       </c>
       <c r="K327" s="14">
-        <v>0.06</v>
+        <v>5.1058246977644828E-2</v>
       </c>
       <c r="L327" s="15">
-        <v>2.5529123488822414</v>
+        <v>0.85097078296074713</v>
       </c>
       <c r="M327" s="7"/>
       <c r="N327" s="7"/>
       <c r="O327" s="7"/>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" s="31" t="s">
         <v>70</v>
       </c>
@@ -14270,7 +14270,7 @@
         <v>16</v>
       </c>
       <c r="F328" s="10">
-        <v>1734</v>
+        <v>578</v>
       </c>
       <c r="G328" s="10">
         <v>0</v>
@@ -14294,7 +14294,7 @@
       <c r="N328" s="7"/>
       <c r="O328" s="7"/>
     </row>
-    <row r="329" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" s="31" t="s">
         <v>70</v>
       </c>
@@ -14311,13 +14311,13 @@
         <v>16</v>
       </c>
       <c r="F329" s="10">
-        <v>9555</v>
+        <v>3185</v>
       </c>
       <c r="G329" s="10">
         <v>5780</v>
       </c>
       <c r="H329" s="11">
-        <v>1.6531141868512111</v>
+        <v>0.55103806228373697</v>
       </c>
       <c r="I329" s="11">
         <v>0.63500000000000001</v>
@@ -14326,16 +14326,16 @@
         <v>0.06</v>
       </c>
       <c r="K329" s="14">
-        <v>0.06</v>
+        <v>5.206658856224286E-2</v>
       </c>
       <c r="L329" s="15">
-        <v>2.6033294281121435</v>
+        <v>0.86777647603738106</v>
       </c>
       <c r="M329" s="7"/>
       <c r="N329" s="7"/>
       <c r="O329" s="7"/>
     </row>
-    <row r="330" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="31" t="s">
         <v>70</v>
       </c>
@@ -14352,7 +14352,7 @@
         <v>16</v>
       </c>
       <c r="F330" s="10">
-        <v>387</v>
+        <v>129</v>
       </c>
       <c r="G330" s="10">
         <v>0</v>
@@ -14376,7 +14376,7 @@
       <c r="N330" s="7"/>
       <c r="O330" s="7"/>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="31" t="s">
         <v>70</v>
       </c>
@@ -14393,13 +14393,13 @@
         <v>16</v>
       </c>
       <c r="F331" s="10">
-        <v>11076</v>
+        <v>3692</v>
       </c>
       <c r="G331" s="10">
         <v>6717</v>
       </c>
       <c r="H331" s="11">
-        <v>1.6489504242965609</v>
+        <v>0.54965014143218693</v>
       </c>
       <c r="I331" s="11">
         <v>0.63500000000000001</v>
@@ -14408,16 +14408,16 @@
         <v>0.06</v>
       </c>
       <c r="K331" s="14">
-        <v>0.06</v>
+        <v>5.1935446434537347E-2</v>
       </c>
       <c r="L331" s="15">
-        <v>2.5967723217268674</v>
+        <v>0.86559077390895578</v>
       </c>
       <c r="M331" s="7"/>
       <c r="N331" s="7"/>
       <c r="O331" s="7"/>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="31" t="s">
         <v>70</v>
       </c>
@@ -14434,7 +14434,7 @@
         <v>16</v>
       </c>
       <c r="F332" s="10">
-        <v>516</v>
+        <v>172</v>
       </c>
       <c r="G332" s="10">
         <v>0</v>
@@ -14458,7 +14458,7 @@
       <c r="N332" s="7"/>
       <c r="O332" s="7"/>
     </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" s="31" t="s">
         <v>70</v>
       </c>
@@ -14475,13 +14475,13 @@
         <v>16</v>
       </c>
       <c r="F333" s="10">
-        <v>5127</v>
+        <v>1709</v>
       </c>
       <c r="G333" s="10">
         <v>3184</v>
       </c>
       <c r="H333" s="11">
-        <v>1.6102386934673367</v>
+        <v>0.53674623115577891</v>
       </c>
       <c r="I333" s="11">
         <v>0.63500000000000001</v>
@@ -14490,16 +14490,16 @@
         <v>0.06</v>
       </c>
       <c r="K333" s="14">
-        <v>0.06</v>
+        <v>5.0716179321805881E-2</v>
       </c>
       <c r="L333" s="15">
-        <v>2.5358089660902938</v>
+        <v>0.84526965536343135</v>
       </c>
       <c r="M333" s="7"/>
       <c r="N333" s="7"/>
       <c r="O333" s="7"/>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" s="31" t="s">
         <v>70</v>
       </c>
@@ -14516,7 +14516,7 @@
         <v>16</v>
       </c>
       <c r="F334" s="10">
-        <v>1101</v>
+        <v>367</v>
       </c>
       <c r="G334" s="10">
         <v>0</v>
@@ -14540,7 +14540,7 @@
       <c r="N334" s="7"/>
       <c r="O334" s="7"/>
     </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" s="31" t="s">
         <v>70</v>
       </c>
@@ -14557,13 +14557,13 @@
         <v>16</v>
       </c>
       <c r="F335" s="10">
-        <v>6063</v>
+        <v>2021</v>
       </c>
       <c r="G335" s="10">
         <v>3658</v>
       </c>
       <c r="H335" s="11">
-        <v>1.6574630945872062</v>
+        <v>0.5524876981957354</v>
       </c>
       <c r="I335" s="11">
         <v>0.63500000000000001</v>
@@ -14572,16 +14572,16 @@
         <v>0.06</v>
       </c>
       <c r="K335" s="14">
-        <v>0.06</v>
+        <v>5.2203562034242708E-2</v>
       </c>
       <c r="L335" s="15">
-        <v>2.6101781017121355</v>
+        <v>0.87005936723737853</v>
       </c>
       <c r="M335" s="7"/>
       <c r="N335" s="7"/>
       <c r="O335" s="7"/>
     </row>
-    <row r="336" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" s="31" t="s">
         <v>70</v>
       </c>
@@ -14598,7 +14598,7 @@
         <v>16</v>
       </c>
       <c r="F336" s="10">
-        <v>498</v>
+        <v>166</v>
       </c>
       <c r="G336" s="10">
         <v>0</v>
@@ -14622,7 +14622,7 @@
       <c r="N336" s="7"/>
       <c r="O336" s="7"/>
     </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" s="31" t="s">
         <v>70</v>
       </c>
@@ -14639,7 +14639,7 @@
         <v>16</v>
       </c>
       <c r="F337" s="10">
-        <v>231</v>
+        <v>77</v>
       </c>
       <c r="G337" s="10">
         <v>0</v>
@@ -14663,7 +14663,7 @@
       <c r="N337" s="7"/>
       <c r="O337" s="7"/>
     </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" s="31" t="s">
         <v>70</v>
       </c>
@@ -14680,7 +14680,7 @@
         <v>16</v>
       </c>
       <c r="F338" s="10">
-        <v>285</v>
+        <v>95</v>
       </c>
       <c r="G338" s="10">
         <v>0</v>
@@ -14704,7 +14704,7 @@
       <c r="N338" s="7"/>
       <c r="O338" s="7"/>
     </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" s="31" t="s">
         <v>70</v>
       </c>
@@ -14721,7 +14721,7 @@
         <v>16</v>
       </c>
       <c r="F339" s="10">
-        <v>318</v>
+        <v>106</v>
       </c>
       <c r="G339" s="10">
         <v>0</v>
@@ -14745,7 +14745,7 @@
       <c r="N339" s="7"/>
       <c r="O339" s="7"/>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" s="31" t="s">
         <v>70</v>
       </c>
@@ -14762,7 +14762,7 @@
         <v>16</v>
       </c>
       <c r="F340" s="10">
-        <v>570</v>
+        <v>190</v>
       </c>
       <c r="G340" s="10">
         <v>0</v>
@@ -14786,7 +14786,7 @@
       <c r="N340" s="7"/>
       <c r="O340" s="7"/>
     </row>
-    <row r="341" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" s="31" t="s">
         <v>70</v>
       </c>
@@ -14803,7 +14803,7 @@
         <v>16</v>
       </c>
       <c r="F341" s="10">
-        <v>519834</v>
+        <v>173278</v>
       </c>
       <c r="G341" s="10">
         <v>0</v>
@@ -14827,7 +14827,7 @@
       <c r="N341" s="7"/>
       <c r="O341" s="7"/>
     </row>
-    <row r="342" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" s="31" t="s">
         <v>72</v>
       </c>
@@ -14868,7 +14868,7 @@
       <c r="N342" s="7"/>
       <c r="O342" s="7"/>
     </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" s="31" t="s">
         <v>72</v>
       </c>
@@ -14909,7 +14909,7 @@
       <c r="N343" s="7"/>
       <c r="O343" s="7"/>
     </row>
-    <row r="344" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" s="31" t="s">
         <v>72</v>
       </c>
@@ -14950,7 +14950,7 @@
       <c r="N344" s="7"/>
       <c r="O344" s="7"/>
     </row>
-    <row r="345" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" s="31" t="s">
         <v>72</v>
       </c>
@@ -14991,7 +14991,7 @@
       <c r="N345" s="7"/>
       <c r="O345" s="7"/>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" s="31" t="s">
         <v>72</v>
       </c>
@@ -15032,7 +15032,7 @@
       <c r="N346" s="7"/>
       <c r="O346" s="7"/>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" s="31" t="s">
         <v>72</v>
       </c>
@@ -15073,7 +15073,7 @@
       <c r="N347" s="7"/>
       <c r="O347" s="7"/>
     </row>
-    <row r="348" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" s="31" t="s">
         <v>72</v>
       </c>
@@ -15114,7 +15114,7 @@
       <c r="N348" s="7"/>
       <c r="O348" s="7"/>
     </row>
-    <row r="349" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" s="31" t="s">
         <v>72</v>
       </c>
@@ -15155,7 +15155,7 @@
       <c r="N349" s="7"/>
       <c r="O349" s="7"/>
     </row>
-    <row r="350" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" s="31" t="s">
         <v>72</v>
       </c>
@@ -15196,7 +15196,7 @@
       <c r="N350" s="7"/>
       <c r="O350" s="7"/>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" s="31" t="s">
         <v>72</v>
       </c>
@@ -15237,7 +15237,7 @@
       <c r="N351" s="7"/>
       <c r="O351" s="7"/>
     </row>
-    <row r="352" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" s="31" t="s">
         <v>72</v>
       </c>
@@ -15278,7 +15278,7 @@
       <c r="N352" s="7"/>
       <c r="O352" s="7"/>
     </row>
-    <row r="353" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" s="31" t="s">
         <v>72</v>
       </c>
@@ -15319,7 +15319,7 @@
       <c r="N353" s="7"/>
       <c r="O353" s="7"/>
     </row>
-    <row r="354" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" s="31" t="s">
         <v>72</v>
       </c>
@@ -15360,7 +15360,7 @@
       <c r="N354" s="7"/>
       <c r="O354" s="7"/>
     </row>
-    <row r="355" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" s="31" t="s">
         <v>72</v>
       </c>
@@ -15401,7 +15401,7 @@
       <c r="N355" s="7"/>
       <c r="O355" s="7"/>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" s="31" t="s">
         <v>72</v>
       </c>
@@ -15442,7 +15442,7 @@
       <c r="N356" s="7"/>
       <c r="O356" s="7"/>
     </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" s="31" t="s">
         <v>72</v>
       </c>
@@ -15483,7 +15483,7 @@
       <c r="N357" s="7"/>
       <c r="O357" s="7"/>
     </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" s="31" t="s">
         <v>72</v>
       </c>
@@ -15524,7 +15524,7 @@
       <c r="N358" s="7"/>
       <c r="O358" s="7"/>
     </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" s="31" t="s">
         <v>74</v>
       </c>
@@ -15565,7 +15565,7 @@
       <c r="N359" s="7"/>
       <c r="O359" s="7"/>
     </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" s="31" t="s">
         <v>74</v>
       </c>
@@ -15606,7 +15606,7 @@
       <c r="N360" s="7"/>
       <c r="O360" s="7"/>
     </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" s="31" t="s">
         <v>74</v>
       </c>
@@ -15647,7 +15647,7 @@
       <c r="N361" s="7"/>
       <c r="O361" s="7"/>
     </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" s="31" t="s">
         <v>74</v>
       </c>
@@ -15688,7 +15688,7 @@
       <c r="N362" s="7"/>
       <c r="O362" s="7"/>
     </row>
-    <row r="363" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" s="31" t="s">
         <v>74</v>
       </c>
@@ -15729,7 +15729,7 @@
       <c r="N363" s="7"/>
       <c r="O363" s="7"/>
     </row>
-    <row r="364" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" s="31" t="s">
         <v>74</v>
       </c>
@@ -15770,7 +15770,7 @@
       <c r="N364" s="7"/>
       <c r="O364" s="7"/>
     </row>
-    <row r="365" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" s="31" t="s">
         <v>74</v>
       </c>
@@ -15811,7 +15811,7 @@
       <c r="N365" s="7"/>
       <c r="O365" s="7"/>
     </row>
-    <row r="366" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" s="31" t="s">
         <v>74</v>
       </c>
@@ -15852,7 +15852,7 @@
       <c r="N366" s="7"/>
       <c r="O366" s="7"/>
     </row>
-    <row r="367" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367" s="31" t="s">
         <v>74</v>
       </c>
@@ -15893,7 +15893,7 @@
       <c r="N367" s="7"/>
       <c r="O367" s="7"/>
     </row>
-    <row r="368" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" s="31" t="s">
         <v>74</v>
       </c>
@@ -15934,7 +15934,7 @@
       <c r="N368" s="7"/>
       <c r="O368" s="7"/>
     </row>
-    <row r="369" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A369" s="31" t="s">
         <v>74</v>
       </c>
@@ -15975,7 +15975,7 @@
       <c r="N369" s="7"/>
       <c r="O369" s="7"/>
     </row>
-    <row r="370" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" s="31" t="s">
         <v>74</v>
       </c>
@@ -16016,7 +16016,7 @@
       <c r="N370" s="7"/>
       <c r="O370" s="7"/>
     </row>
-    <row r="371" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" s="31" t="s">
         <v>74</v>
       </c>
@@ -16057,7 +16057,7 @@
       <c r="N371" s="7"/>
       <c r="O371" s="7"/>
     </row>
-    <row r="372" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" s="31" t="s">
         <v>74</v>
       </c>
@@ -16098,7 +16098,7 @@
       <c r="N372" s="7"/>
       <c r="O372" s="7"/>
     </row>
-    <row r="373" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" s="31" t="s">
         <v>74</v>
       </c>
@@ -16139,7 +16139,7 @@
       <c r="N373" s="7"/>
       <c r="O373" s="7"/>
     </row>
-    <row r="374" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A374" s="31" t="s">
         <v>74</v>
       </c>
@@ -16180,7 +16180,7 @@
       <c r="N374" s="7"/>
       <c r="O374" s="7"/>
     </row>
-    <row r="375" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" s="31" t="s">
         <v>74</v>
       </c>
@@ -16654,7 +16654,13 @@
       <c r="O402" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L375" xr:uid="{301DFA57-F574-41A6-870E-2EAA91A7C829}"/>
+  <autoFilter ref="A1:L375" xr:uid="{301DFA57-F574-41A6-870E-2EAA91A7C829}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1.-Porcentaje de centros de salud autoevaluados mediante MAIS"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="E2:E375" xr:uid="{03D98A79-4A49-443A-9A5F-37BFDA6F5BA4}"/>
   </dataValidations>

</xml_diff>